<commit_message>
Created Verfiy  Cloumn Header Name and column filter
</commit_message>
<xml_diff>
--- a/src/test/resources/DataOfPIA.xlsx
+++ b/src/test/resources/DataOfPIA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raju.yadav\eclipse-workspace\PIA\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raju.yadav\eclipse-workspace\git\PIA_project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E382BC6-5CF9-43ED-A458-F915E2FCA74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF2161-5353-4846-AF05-26236DC538AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B36F36BC-1B29-44FC-BF98-46D97024B774}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="149">
   <si>
     <t>Sr no</t>
   </si>
@@ -486,12 +486,18 @@
     <t>Password Must Have Some Value
 Password Does Not Match!</t>
   </si>
+  <si>
+    <t>VerifyTC028_Verify_ColumnHeaderNames</t>
+  </si>
+  <si>
+    <t>TC028</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +538,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -553,7 +566,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -561,12 +574,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,6 +637,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -944,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB98528B-91D9-4A38-90A7-5695A0BACC85}">
-  <dimension ref="A1:AC27"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K10" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,6 +2106,70 @@
         <v>140</v>
       </c>
     </row>
+    <row r="28" spans="1:29" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2110,6 +2205,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bd38acd0-b5ef-4f26-ad5a-4b4211772be7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6C221BDF4319C4E86CD8A3A6CF15EF6" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb0efa730961560f7c1dfb380fc877d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bd38acd0-b5ef-4f26-ad5a-4b4211772be7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4e358320858bdeef49ab313120809b2" ns3:_="">
     <xsd:import namespace="bd38acd0-b5ef-4f26-ad5a-4b4211772be7"/>
@@ -2265,24 +2377,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EFF498-18A4-441F-A598-CEE55528C0BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bd38acd0-b5ef-4f26-ad5a-4b4211772be7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bd38acd0-b5ef-4f26-ad5a-4b4211772be7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D981EB97-C459-4263-A19F-79ED0A74CA35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{976EBD47-1E41-4C70-B92F-0B861858E44A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2298,28 +2417,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D981EB97-C459-4263-A19F-79ED0A74CA35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EFF498-18A4-441F-A598-CEE55528C0BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bd38acd0-b5ef-4f26-ad5a-4b4211772be7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>